<commit_message>
Adding the converted GIS data for Scotland
Added 2010 & 2011 midyr population estimates
Added dzone & izone shape files (converted from ngrid to degrees)
</commit_message>
<xml_diff>
--- a/sds2011.xlsx
+++ b/sds2011.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="10980" windowHeight="4725"/>
+    <workbookView xWindow="120" yWindow="100" windowWidth="24160" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="prevelence" sheetId="19" r:id="rId1"/>
     <sheet name="fact" sheetId="14" r:id="rId2"/>
-    <sheet name="summarymatrix" sheetId="11" r:id="rId3"/>
+    <sheet name="summary" sheetId="11" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fact!$A$1:$C$127</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="125">
   <si>
     <t>metric</t>
   </si>
@@ -392,19 +396,22 @@
   </si>
   <si>
     <t>q0</t>
+  </si>
+  <si>
+    <t>Scotland</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +440,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -442,7 +465,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -455,14 +478,14 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -471,44 +494,83 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -540,12 +602,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -580,9 +636,28 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -879,29 +954,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -913,504 +988,538 @@
       <c r="F1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="27" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="33">
         <v>2221</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="33">
         <v>17919</v>
       </c>
-      <c r="F2" s="35">
+      <c r="F2" s="33">
         <v>35</v>
       </c>
-      <c r="G2" s="36">
+      <c r="G2" s="34">
         <f>SUM(D2:F2)</f>
         <v>20175</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="35">
         <v>366860</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="18">
         <v>55.566175687500007</v>
       </c>
-      <c r="J2" s="30">
+      <c r="J2" s="28">
         <v>-4.609001654166665</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="33">
         <v>614</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="33">
         <v>4846</v>
       </c>
-      <c r="F3" s="35">
+      <c r="F3" s="33">
         <v>33</v>
       </c>
-      <c r="G3" s="36">
+      <c r="G3" s="34">
         <f t="shared" ref="G3:G15" si="0">SUM(D3:F3)</f>
         <v>5493</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="35">
         <v>112870</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="18">
         <v>55.60719344615385</v>
       </c>
-      <c r="J3" s="30">
+      <c r="J3" s="28">
         <v>-2.7004535461538461</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="33">
         <v>893</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="33">
         <v>7236</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="33">
         <v>39</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="34">
         <f t="shared" si="0"/>
         <v>8168</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="35">
         <v>148190</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="18">
         <v>55.027784740932674</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="28">
         <v>-3.8202527512953344</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="33">
         <v>1969</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="33">
         <v>16164</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="33">
         <v>59</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="34">
         <f t="shared" si="0"/>
         <v>18192</v>
       </c>
-      <c r="H5" s="37">
+      <c r="H5" s="35">
         <v>364945</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="18">
         <v>56.163072748344334</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="28">
         <v>-3.2001611412803546</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="33">
         <v>1606</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="33">
         <v>12528</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="33">
         <v>67</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="34">
         <f t="shared" si="0"/>
         <v>14201</v>
       </c>
-      <c r="H6" s="37">
+      <c r="H6" s="35">
         <v>293386</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="18">
         <v>56.064990280323407</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="28">
         <v>-3.8520161617250697</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="33">
         <v>3053</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="33">
         <v>20902</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="33">
         <v>85</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="34">
         <f t="shared" si="0"/>
         <v>24040</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="35">
         <v>550620</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="18">
         <v>57.306753697368443</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="28">
         <v>-2.39230568859649</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="33">
         <v>6180</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="33">
         <v>50005</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="33">
         <v>527</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="34">
         <f t="shared" si="0"/>
         <v>56712</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H8" s="35">
         <v>1203870</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="18">
         <v>55.868988067209798</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="28">
         <v>-4.3449574005431044</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="33">
         <v>1758</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="33">
         <v>12479</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="33">
         <v>128</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="34">
         <f t="shared" si="0"/>
         <v>14365</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9" s="35">
         <v>310830</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="18">
         <v>57.144289492753657</v>
       </c>
-      <c r="J9" s="30">
+      <c r="J9" s="28">
         <v>-4.5762839468599044</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="33">
         <v>3513</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="33">
         <v>24998</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="33">
         <v>118</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="34">
         <f t="shared" si="0"/>
         <v>28629</v>
       </c>
-      <c r="H10" s="37">
+      <c r="H10" s="35">
         <v>562477</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="18">
         <v>55.802350703856774</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J10" s="28">
         <v>-4.0026567245179079</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="33">
         <v>4175</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="33">
         <v>29551</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="33">
         <v>298</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="34">
         <f t="shared" si="0"/>
         <v>34024</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="35">
         <v>836711</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="18">
         <v>55.926776633064541</v>
       </c>
-      <c r="J11" s="30">
+      <c r="J11" s="28">
         <v>-3.2422757217741895</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="33">
         <v>120</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="33">
         <v>853</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="33">
         <v>0</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="34">
         <f t="shared" si="0"/>
         <v>973</v>
       </c>
-      <c r="H12" s="37">
+      <c r="H12" s="35">
         <v>20110</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="18">
         <v>59.000222259259267</v>
       </c>
-      <c r="J12" s="30">
+      <c r="J12" s="28">
         <v>-3.0264093703703705</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="33">
         <v>124</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="33">
         <v>871</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="33">
         <v>4</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="34">
         <f t="shared" si="0"/>
         <v>999</v>
       </c>
-      <c r="H13" s="37">
+      <c r="H13" s="35">
         <v>22400</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="18">
         <v>60.220431733333349</v>
       </c>
-      <c r="J13" s="30">
+      <c r="J13" s="28">
         <v>-1.2161150666666667</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="33">
         <v>1864</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="33">
         <v>18104</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="33">
         <v>98</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="34">
         <f t="shared" si="0"/>
         <v>20066</v>
       </c>
-      <c r="H14" s="37">
+      <c r="H14" s="35">
         <v>402641</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="18">
         <v>56.496416473790269</v>
       </c>
-      <c r="J14" s="30">
+      <c r="J14" s="28">
         <v>-3.0871150322580667</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="36">
         <v>182</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="36">
         <v>1058</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="36">
         <v>1</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G15" s="37">
         <f t="shared" si="0"/>
         <v>1241</v>
       </c>
-      <c r="H15" s="40">
+      <c r="H15" s="38">
         <v>26190</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="25">
         <v>57.991980777777776</v>
       </c>
-      <c r="J15" s="31">
+      <c r="J15" s="29">
         <v>-6.6767360833333322</v>
       </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="39"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="42">
+        <f t="shared" ref="D16:H16" si="1">SUM(D2:D15)</f>
+        <v>28272</v>
+      </c>
+      <c r="E16" s="42">
+        <f t="shared" si="1"/>
+        <v>217514</v>
+      </c>
+      <c r="F16" s="42">
+        <f t="shared" si="1"/>
+        <v>1492</v>
+      </c>
+      <c r="G16" s="44">
+        <f t="shared" si="1"/>
+        <v>247278</v>
+      </c>
+      <c r="H16" s="42">
+        <f t="shared" si="1"/>
+        <v>5222100</v>
+      </c>
+      <c r="I16" s="40"/>
+      <c r="J16" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="45.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="18" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="9.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1">
@@ -1420,16 +1529,16 @@
       <c r="B1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1440,7 +1549,7 @@
       <c r="B2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="30" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1451,7 +1560,7 @@
       <c r="B3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1462,7 +1571,7 @@
       <c r="B4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="30" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1473,7 +1582,7 @@
       <c r="B5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="30" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1484,7 +1593,7 @@
       <c r="B6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="30" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1495,7 +1604,7 @@
       <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="30" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1506,7 +1615,7 @@
       <c r="B8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="30" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1517,7 +1626,7 @@
       <c r="B9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="30" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1528,7 +1637,7 @@
       <c r="B10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="30" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1539,7 +1648,7 @@
       <c r="B11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="30" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1550,7 +1659,7 @@
       <c r="B12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="30" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1561,7 +1670,7 @@
       <c r="B13" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="30" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1572,20 +1681,22 @@
       <c r="B14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="30" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:6" s="2" customFormat="1">
+      <c r="A15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="24" t="s">
         <v>98</v>
       </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
@@ -1594,563 +1705,570 @@
       <c r="B16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="30" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="30" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="30" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="30" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="30" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="30" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:6" s="2" customFormat="1">
+      <c r="A29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="24" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="C30" s="32"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="C31" s="32"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="C32" s="32"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="C30" s="30"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="C31" s="30"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="C32" s="30"/>
     </row>
     <row r="33" spans="3:4">
-      <c r="C33" s="32"/>
+      <c r="C33" s="30"/>
     </row>
     <row r="34" spans="3:4">
-      <c r="C34" s="32"/>
+      <c r="C34" s="30"/>
     </row>
     <row r="35" spans="3:4">
-      <c r="C35" s="32"/>
+      <c r="C35" s="30"/>
     </row>
     <row r="36" spans="3:4">
-      <c r="C36" s="32"/>
+      <c r="C36" s="30"/>
     </row>
     <row r="37" spans="3:4">
-      <c r="C37" s="32"/>
+      <c r="C37" s="30"/>
     </row>
     <row r="38" spans="3:4">
-      <c r="C38" s="32"/>
+      <c r="C38" s="30"/>
     </row>
     <row r="39" spans="3:4">
-      <c r="C39" s="32"/>
+      <c r="C39" s="30"/>
     </row>
     <row r="40" spans="3:4">
-      <c r="C40" s="32"/>
+      <c r="C40" s="30"/>
     </row>
     <row r="41" spans="3:4">
-      <c r="C41" s="32"/>
+      <c r="C41" s="30"/>
     </row>
     <row r="42" spans="3:4">
-      <c r="C42" s="32"/>
+      <c r="C42" s="30"/>
     </row>
     <row r="43" spans="3:4">
-      <c r="C43" s="32"/>
+      <c r="C43" s="30"/>
     </row>
     <row r="44" spans="3:4">
-      <c r="C44" s="32"/>
-      <c r="D44" s="15"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="13"/>
     </row>
     <row r="45" spans="3:4">
-      <c r="C45" s="32"/>
-      <c r="D45" s="15"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="13"/>
     </row>
     <row r="46" spans="3:4">
-      <c r="C46" s="32"/>
-      <c r="D46" s="15"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="13"/>
     </row>
     <row r="47" spans="3:4">
-      <c r="C47" s="32"/>
-      <c r="D47" s="15"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="13"/>
     </row>
     <row r="48" spans="3:4">
-      <c r="C48" s="32"/>
-      <c r="D48" s="15"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="13"/>
     </row>
     <row r="49" spans="3:4">
-      <c r="C49" s="32"/>
-      <c r="D49" s="15"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="13"/>
     </row>
     <row r="50" spans="3:4">
-      <c r="C50" s="32"/>
+      <c r="C50" s="30"/>
     </row>
     <row r="51" spans="3:4">
-      <c r="C51" s="32"/>
+      <c r="C51" s="30"/>
     </row>
     <row r="52" spans="3:4">
-      <c r="C52" s="32"/>
+      <c r="C52" s="30"/>
     </row>
     <row r="53" spans="3:4">
-      <c r="C53" s="32"/>
+      <c r="C53" s="30"/>
     </row>
     <row r="54" spans="3:4">
-      <c r="C54" s="32"/>
+      <c r="C54" s="30"/>
     </row>
     <row r="55" spans="3:4">
-      <c r="C55" s="32"/>
+      <c r="C55" s="30"/>
     </row>
     <row r="56" spans="3:4">
-      <c r="C56" s="32"/>
+      <c r="C56" s="30"/>
     </row>
     <row r="57" spans="3:4">
-      <c r="C57" s="32"/>
+      <c r="C57" s="30"/>
     </row>
     <row r="58" spans="3:4">
-      <c r="C58" s="32"/>
+      <c r="C58" s="30"/>
     </row>
     <row r="59" spans="3:4">
-      <c r="C59" s="32"/>
+      <c r="C59" s="30"/>
     </row>
     <row r="60" spans="3:4">
-      <c r="C60" s="32"/>
+      <c r="C60" s="30"/>
     </row>
     <row r="61" spans="3:4">
-      <c r="C61" s="32"/>
+      <c r="C61" s="30"/>
     </row>
     <row r="62" spans="3:4">
-      <c r="C62" s="32"/>
+      <c r="C62" s="30"/>
     </row>
     <row r="63" spans="3:4">
-      <c r="C63" s="32"/>
+      <c r="C63" s="30"/>
     </row>
     <row r="64" spans="3:4">
-      <c r="C64" s="32"/>
+      <c r="C64" s="30"/>
     </row>
     <row r="65" spans="3:3">
-      <c r="C65" s="32"/>
+      <c r="C65" s="30"/>
     </row>
     <row r="66" spans="3:3">
-      <c r="C66" s="32"/>
+      <c r="C66" s="30"/>
     </row>
     <row r="67" spans="3:3">
-      <c r="C67" s="32"/>
+      <c r="C67" s="30"/>
     </row>
     <row r="68" spans="3:3">
-      <c r="C68" s="32"/>
+      <c r="C68" s="30"/>
     </row>
     <row r="69" spans="3:3">
-      <c r="C69" s="32"/>
+      <c r="C69" s="30"/>
     </row>
     <row r="70" spans="3:3">
-      <c r="C70" s="32"/>
+      <c r="C70" s="30"/>
     </row>
     <row r="71" spans="3:3">
-      <c r="C71" s="32"/>
+      <c r="C71" s="30"/>
     </row>
     <row r="72" spans="3:3">
-      <c r="C72" s="32"/>
+      <c r="C72" s="30"/>
     </row>
     <row r="73" spans="3:3">
-      <c r="C73" s="32"/>
+      <c r="C73" s="30"/>
     </row>
     <row r="74" spans="3:3">
-      <c r="C74" s="32"/>
+      <c r="C74" s="30"/>
     </row>
     <row r="75" spans="3:3">
-      <c r="C75" s="32"/>
+      <c r="C75" s="30"/>
     </row>
     <row r="76" spans="3:3">
-      <c r="C76" s="32"/>
+      <c r="C76" s="30"/>
     </row>
     <row r="77" spans="3:3">
-      <c r="C77" s="32"/>
+      <c r="C77" s="30"/>
     </row>
     <row r="78" spans="3:3">
-      <c r="C78" s="32"/>
+      <c r="C78" s="30"/>
     </row>
     <row r="79" spans="3:3">
-      <c r="C79" s="32"/>
+      <c r="C79" s="30"/>
     </row>
     <row r="80" spans="3:3">
-      <c r="C80" s="32"/>
+      <c r="C80" s="30"/>
     </row>
     <row r="81" spans="2:5">
-      <c r="C81" s="32"/>
+      <c r="C81" s="30"/>
     </row>
     <row r="82" spans="2:5">
-      <c r="C82" s="32"/>
+      <c r="C82" s="30"/>
     </row>
     <row r="83" spans="2:5">
-      <c r="C83" s="32"/>
+      <c r="C83" s="30"/>
     </row>
     <row r="84" spans="2:5">
-      <c r="C84" s="32"/>
+      <c r="C84" s="30"/>
     </row>
     <row r="85" spans="2:5">
-      <c r="C85" s="32"/>
+      <c r="C85" s="30"/>
     </row>
     <row r="86" spans="2:5">
-      <c r="B86" s="15"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="33"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="30"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="31"/>
     </row>
     <row r="87" spans="2:5">
-      <c r="B87" s="15"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="33"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="31"/>
     </row>
     <row r="88" spans="2:5">
-      <c r="B88" s="15"/>
-      <c r="C88" s="32"/>
-      <c r="D88" s="15"/>
-      <c r="E88" s="33"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="31"/>
     </row>
     <row r="89" spans="2:5">
-      <c r="B89" s="15"/>
-      <c r="C89" s="32"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="33"/>
+      <c r="B89" s="13"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="31"/>
     </row>
     <row r="90" spans="2:5">
-      <c r="B90" s="15"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="33"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="31"/>
     </row>
     <row r="91" spans="2:5">
-      <c r="B91" s="15"/>
-      <c r="C91" s="32"/>
-      <c r="D91" s="15"/>
-      <c r="E91" s="33"/>
+      <c r="B91" s="13"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="31"/>
     </row>
     <row r="92" spans="2:5">
-      <c r="B92" s="15"/>
-      <c r="C92" s="32"/>
-      <c r="D92" s="15"/>
-      <c r="E92" s="33"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="31"/>
     </row>
     <row r="93" spans="2:5">
-      <c r="B93" s="15"/>
-      <c r="C93" s="32"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="33"/>
+      <c r="B93" s="13"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="31"/>
     </row>
     <row r="94" spans="2:5">
-      <c r="B94" s="15"/>
-      <c r="C94" s="32"/>
-      <c r="D94" s="15"/>
-      <c r="E94" s="33"/>
+      <c r="B94" s="13"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="31"/>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="15"/>
-      <c r="C95" s="32"/>
-      <c r="D95" s="15"/>
-      <c r="E95" s="33"/>
+      <c r="B95" s="13"/>
+      <c r="C95" s="30"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="31"/>
     </row>
     <row r="96" spans="2:5">
-      <c r="B96" s="15"/>
-      <c r="C96" s="32"/>
-      <c r="D96" s="15"/>
-      <c r="E96" s="33"/>
+      <c r="B96" s="13"/>
+      <c r="C96" s="30"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="31"/>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="15"/>
-      <c r="C97" s="32"/>
-      <c r="D97" s="15"/>
-      <c r="E97" s="33"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="31"/>
     </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="15"/>
-      <c r="C98" s="32"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="33"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="30"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="31"/>
     </row>
     <row r="99" spans="2:5">
-      <c r="B99" s="15"/>
-      <c r="C99" s="32"/>
-      <c r="D99" s="15"/>
-      <c r="E99" s="33"/>
+      <c r="B99" s="13"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="31"/>
     </row>
     <row r="100" spans="2:5">
-      <c r="B100" s="15"/>
-      <c r="C100" s="32"/>
-      <c r="D100" s="15"/>
-      <c r="E100" s="33"/>
+      <c r="B100" s="13"/>
+      <c r="C100" s="30"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="31"/>
     </row>
     <row r="101" spans="2:5">
-      <c r="B101" s="15"/>
-      <c r="C101" s="32"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="33"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="30"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="31"/>
     </row>
     <row r="102" spans="2:5">
-      <c r="B102" s="15"/>
-      <c r="C102" s="32"/>
-      <c r="D102" s="15"/>
-      <c r="E102" s="33"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="30"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="31"/>
     </row>
     <row r="103" spans="2:5">
-      <c r="B103" s="15"/>
-      <c r="C103" s="32"/>
-      <c r="D103" s="15"/>
-      <c r="E103" s="33"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="30"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="31"/>
     </row>
     <row r="104" spans="2:5">
-      <c r="B104" s="15"/>
-      <c r="C104" s="32"/>
-      <c r="D104" s="15"/>
-      <c r="E104" s="33"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="30"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="31"/>
     </row>
     <row r="105" spans="2:5">
-      <c r="B105" s="15"/>
-      <c r="C105" s="32"/>
-      <c r="D105" s="15"/>
-      <c r="E105" s="33"/>
+      <c r="B105" s="13"/>
+      <c r="C105" s="30"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="31"/>
     </row>
     <row r="106" spans="2:5">
-      <c r="B106" s="15"/>
-      <c r="C106" s="32"/>
-      <c r="D106" s="15"/>
-      <c r="E106" s="33"/>
+      <c r="B106" s="13"/>
+      <c r="C106" s="30"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="31"/>
     </row>
     <row r="107" spans="2:5">
-      <c r="B107" s="15"/>
-      <c r="C107" s="32"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="33"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="30"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="31"/>
     </row>
     <row r="108" spans="2:5">
-      <c r="B108" s="15"/>
-      <c r="C108" s="32"/>
-      <c r="D108" s="15"/>
-      <c r="E108" s="33"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="30"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="31"/>
     </row>
     <row r="109" spans="2:5">
-      <c r="B109" s="15"/>
-      <c r="C109" s="32"/>
-      <c r="D109" s="15"/>
-      <c r="E109" s="33"/>
+      <c r="B109" s="13"/>
+      <c r="C109" s="30"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="31"/>
     </row>
     <row r="110" spans="2:5">
-      <c r="B110" s="15"/>
-      <c r="C110" s="32"/>
-      <c r="D110" s="15"/>
-      <c r="E110" s="33"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="30"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="31"/>
     </row>
     <row r="111" spans="2:5">
-      <c r="B111" s="15"/>
-      <c r="C111" s="32"/>
-      <c r="D111" s="15"/>
-      <c r="E111" s="33"/>
+      <c r="B111" s="13"/>
+      <c r="C111" s="30"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="31"/>
     </row>
     <row r="112" spans="2:5">
-      <c r="B112" s="15"/>
-      <c r="C112" s="32"/>
-      <c r="D112" s="15"/>
-      <c r="E112" s="33"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="30"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="31"/>
     </row>
     <row r="113" spans="2:5">
-      <c r="B113" s="15"/>
-      <c r="C113" s="32"/>
-      <c r="D113" s="15"/>
-      <c r="E113" s="33"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="30"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="31"/>
     </row>
     <row r="114" spans="2:5">
-      <c r="C114" s="32"/>
+      <c r="C114" s="30"/>
     </row>
     <row r="115" spans="2:5">
-      <c r="C115" s="32"/>
+      <c r="C115" s="30"/>
     </row>
     <row r="116" spans="2:5">
-      <c r="C116" s="32"/>
+      <c r="C116" s="30"/>
     </row>
     <row r="117" spans="2:5">
-      <c r="C117" s="32"/>
+      <c r="C117" s="30"/>
     </row>
     <row r="118" spans="2:5">
-      <c r="C118" s="32"/>
+      <c r="C118" s="30"/>
     </row>
     <row r="119" spans="2:5">
-      <c r="C119" s="32"/>
+      <c r="C119" s="30"/>
     </row>
     <row r="120" spans="2:5">
-      <c r="C120" s="32"/>
+      <c r="C120" s="30"/>
     </row>
     <row r="121" spans="2:5">
-      <c r="C121" s="32"/>
+      <c r="C121" s="30"/>
     </row>
     <row r="122" spans="2:5">
-      <c r="C122" s="32"/>
+      <c r="C122" s="30"/>
     </row>
     <row r="123" spans="2:5">
-      <c r="C123" s="32"/>
+      <c r="C123" s="30"/>
     </row>
     <row r="124" spans="2:5">
-      <c r="C124" s="32"/>
+      <c r="C124" s="30"/>
     </row>
     <row r="125" spans="2:5">
-      <c r="C125" s="32"/>
+      <c r="C125" s="30"/>
     </row>
     <row r="126" spans="2:5">
-      <c r="C126" s="32"/>
+      <c r="C126" s="30"/>
     </row>
     <row r="127" spans="2:5">
-      <c r="C127" s="32"/>
+      <c r="C127" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="126" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="126" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="15" width="12.42578125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" style="6" customWidth="1"/>
-    <col min="17" max="25" width="12.42578125" style="12" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="2" width="56.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="12.5" style="5" customWidth="1"/>
+    <col min="16" max="16" width="12.5" style="6" customWidth="1"/>
+    <col min="17" max="25" width="12.5" style="12" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="3" customFormat="1">
@@ -2269,7 +2387,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="10"/>
-      <c r="D3" s="19"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -2299,7 +2417,75 @@
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="C4">
+        <v>0.6</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <v>0.6</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>0.6</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <v>0.6</v>
+      </c>
+      <c r="J4">
+        <v>0.6</v>
+      </c>
+      <c r="K4">
+        <v>0.6</v>
+      </c>
+      <c r="L4">
+        <v>0.5</v>
+      </c>
+      <c r="M4">
+        <v>0.6</v>
+      </c>
+      <c r="N4">
+        <v>0.6</v>
+      </c>
+      <c r="O4">
+        <v>0.5</v>
+      </c>
+      <c r="P4" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="Q4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>0.7</v>
+      </c>
+      <c r="S4">
+        <v>0.6</v>
+      </c>
+      <c r="T4">
+        <v>0.6</v>
+      </c>
+      <c r="U4">
+        <v>0.5</v>
+      </c>
+      <c r="V4">
+        <v>0.5</v>
+      </c>
+      <c r="W4">
+        <v>0.6</v>
+      </c>
+      <c r="X4">
+        <v>0.6</v>
+      </c>
+      <c r="Y4">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="4">
@@ -2308,20 +2494,75 @@
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="14"/>
+      <c r="C5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D5">
+        <v>4.3</v>
+      </c>
+      <c r="E5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G5">
+        <v>4.3</v>
+      </c>
+      <c r="H5">
+        <v>4.2</v>
+      </c>
+      <c r="I5">
+        <v>3.8</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L5">
+        <v>3.5</v>
+      </c>
+      <c r="M5">
+        <v>4.2</v>
+      </c>
+      <c r="N5">
+        <v>3.9</v>
+      </c>
+      <c r="O5">
+        <v>4.5</v>
+      </c>
+      <c r="P5" s="49">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>3.5</v>
+      </c>
+      <c r="R5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="S5">
+        <v>4.2</v>
+      </c>
+      <c r="T5">
+        <v>4.3</v>
+      </c>
+      <c r="U5">
+        <v>3.5</v>
+      </c>
+      <c r="V5">
+        <v>4</v>
+      </c>
+      <c r="W5">
+        <v>4.3</v>
+      </c>
+      <c r="X5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Y5">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="4">
@@ -2330,16 +2571,106 @@
       <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="A7" s="4">
+      <c r="C6">
+        <v>0.9</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1.6</v>
+      </c>
+      <c r="F6">
+        <v>0.7</v>
+      </c>
+      <c r="G6">
+        <v>0.7</v>
+      </c>
+      <c r="H6">
+        <v>0.8</v>
+      </c>
+      <c r="I6">
+        <v>0.9</v>
+      </c>
+      <c r="J6">
+        <v>1.9</v>
+      </c>
+      <c r="K6">
+        <v>0.8</v>
+      </c>
+      <c r="L6">
+        <v>0.9</v>
+      </c>
+      <c r="M6">
+        <v>1.3</v>
+      </c>
+      <c r="N6">
+        <v>1.9</v>
+      </c>
+      <c r="O6">
+        <v>0.9</v>
+      </c>
+      <c r="P6" s="49">
+        <v>2.7</v>
+      </c>
+      <c r="Q6">
+        <v>0.7</v>
+      </c>
+      <c r="R6">
+        <v>2.7</v>
+      </c>
+      <c r="S6">
+        <v>1.2</v>
+      </c>
+      <c r="T6">
+        <v>0.9</v>
+      </c>
+      <c r="U6">
+        <v>0.7</v>
+      </c>
+      <c r="V6">
+        <v>0.8</v>
+      </c>
+      <c r="W6">
+        <v>0.9</v>
+      </c>
+      <c r="X6">
+        <v>1.5</v>
+      </c>
+      <c r="Y6">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="2" customFormat="1">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="4">
@@ -2348,7 +2679,7 @@
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="4">
@@ -2357,7 +2688,7 @@
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="4">
@@ -2366,7 +2697,7 @@
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="4">
@@ -2375,7 +2706,7 @@
       <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="4">
@@ -2384,7 +2715,7 @@
       <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="4">
@@ -2393,7 +2724,7 @@
       <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="4">
@@ -2402,7 +2733,7 @@
       <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="4">
@@ -2411,7 +2742,7 @@
       <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="4">
@@ -2420,9 +2751,9 @@
       <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="32"/>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2430,7 +2761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2438,7 +2769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2446,7 +2777,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2454,7 +2785,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2462,7 +2793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2470,7 +2801,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2478,7 +2809,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2486,7 +2817,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2494,7 +2825,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -2502,7 +2833,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -2510,7 +2841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -2518,7 +2849,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -2526,7 +2857,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -2534,23 +2865,161 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31">
+        <v>25.4</v>
+      </c>
+      <c r="D31">
+        <v>29.6</v>
+      </c>
+      <c r="E31">
+        <v>27.7</v>
+      </c>
+      <c r="F31">
+        <v>25.9</v>
+      </c>
+      <c r="G31">
+        <v>23.4</v>
+      </c>
+      <c r="H31">
+        <v>22.5</v>
+      </c>
+      <c r="I31">
+        <v>23.1</v>
+      </c>
+      <c r="J31">
+        <v>25.1</v>
+      </c>
+      <c r="K31">
+        <v>26.4</v>
+      </c>
+      <c r="L31">
+        <v>23.2</v>
+      </c>
+      <c r="M31">
+        <v>29.1</v>
+      </c>
+      <c r="N31">
+        <v>32.1</v>
+      </c>
+      <c r="O31">
+        <v>23.3</v>
+      </c>
+      <c r="P31" s="49">
+        <v>24.2</v>
+      </c>
+      <c r="Q31">
+        <v>22.5</v>
+      </c>
+      <c r="R31">
+        <v>32.1</v>
+      </c>
+      <c r="S31">
+        <v>25.8</v>
+      </c>
+      <c r="T31">
+        <v>25.3</v>
+      </c>
+      <c r="U31">
+        <v>22.5</v>
+      </c>
+      <c r="V31">
+        <v>23.3</v>
+      </c>
+      <c r="W31">
+        <v>25.3</v>
+      </c>
+      <c r="X31">
+        <v>27.4</v>
+      </c>
+      <c r="Y31">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32">
+        <v>54.8</v>
+      </c>
+      <c r="D32">
+        <v>55.6</v>
+      </c>
+      <c r="E32">
+        <v>55</v>
+      </c>
+      <c r="F32">
+        <v>58.7</v>
+      </c>
+      <c r="G32">
+        <v>57.4</v>
+      </c>
+      <c r="H32">
+        <v>54.7</v>
+      </c>
+      <c r="I32">
+        <v>53.1</v>
+      </c>
+      <c r="J32">
+        <v>55.2</v>
+      </c>
+      <c r="K32">
+        <v>56.7</v>
+      </c>
+      <c r="L32">
+        <v>56</v>
+      </c>
+      <c r="M32">
+        <v>60.3</v>
+      </c>
+      <c r="N32">
+        <v>60.9</v>
+      </c>
+      <c r="O32">
+        <v>55.5</v>
+      </c>
+      <c r="P32" s="49">
+        <v>57.5</v>
+      </c>
+      <c r="Q32">
+        <v>53.1</v>
+      </c>
+      <c r="R32">
+        <v>60.9</v>
+      </c>
+      <c r="S32">
+        <v>56.5</v>
+      </c>
+      <c r="T32">
+        <v>55.8</v>
+      </c>
+      <c r="U32">
+        <v>53.1</v>
+      </c>
+      <c r="V32">
+        <v>55.1</v>
+      </c>
+      <c r="W32">
+        <v>55.8</v>
+      </c>
+      <c r="X32">
+        <v>57.5</v>
+      </c>
+      <c r="Y32">
+        <v>60.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2558,7 +3027,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -2566,23 +3035,161 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35">
+        <v>37.6</v>
+      </c>
+      <c r="D35">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E35">
+        <v>32</v>
+      </c>
+      <c r="F35">
+        <v>37.9</v>
+      </c>
+      <c r="G35">
+        <v>40.9</v>
+      </c>
+      <c r="H35">
+        <v>46.9</v>
+      </c>
+      <c r="I35">
+        <v>35.6</v>
+      </c>
+      <c r="J35">
+        <v>36.4</v>
+      </c>
+      <c r="K35">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="L35">
+        <v>31.1</v>
+      </c>
+      <c r="M35">
+        <v>33.6</v>
+      </c>
+      <c r="N35">
+        <v>26.7</v>
+      </c>
+      <c r="O35">
+        <v>43.6</v>
+      </c>
+      <c r="P35" s="49">
+        <v>40</v>
+      </c>
+      <c r="Q35">
+        <v>26.7</v>
+      </c>
+      <c r="R35">
+        <v>46.9</v>
+      </c>
+      <c r="S35">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="T35">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="U35">
+        <v>26.7</v>
+      </c>
+      <c r="V35">
+        <v>33.9</v>
+      </c>
+      <c r="W35">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="X35">
+        <v>39.5</v>
+      </c>
+      <c r="Y35">
+        <v>46.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36">
+        <v>13.4</v>
+      </c>
+      <c r="D36">
+        <v>11.5</v>
+      </c>
+      <c r="E36">
+        <v>12.2</v>
+      </c>
+      <c r="F36">
+        <v>13</v>
+      </c>
+      <c r="G36">
+        <v>14.3</v>
+      </c>
+      <c r="H36">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="I36">
+        <v>16.2</v>
+      </c>
+      <c r="J36">
+        <v>14.9</v>
+      </c>
+      <c r="K36">
+        <v>14.7</v>
+      </c>
+      <c r="L36">
+        <v>12.7</v>
+      </c>
+      <c r="M36">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="N36">
+        <v>14.4</v>
+      </c>
+      <c r="O36">
+        <v>14.8</v>
+      </c>
+      <c r="P36" s="49">
+        <v>18.3</v>
+      </c>
+      <c r="Q36">
+        <v>11.5</v>
+      </c>
+      <c r="R36">
+        <v>18.3</v>
+      </c>
+      <c r="S36">
+        <v>14.6</v>
+      </c>
+      <c r="T36">
+        <v>14.6</v>
+      </c>
+      <c r="U36">
+        <v>11.5</v>
+      </c>
+      <c r="V36">
+        <v>13.1</v>
+      </c>
+      <c r="W36">
+        <v>14.6</v>
+      </c>
+      <c r="X36">
+        <v>15.9</v>
+      </c>
+      <c r="Y36">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2590,7 +3197,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -2598,7 +3205,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -2606,7 +3213,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -2614,7 +3221,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -2622,7 +3229,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -2630,7 +3237,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -2638,7 +3245,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -2646,7 +3253,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -2654,7 +3261,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -2662,7 +3269,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -2670,7 +3277,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -2728,6 +3335,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="126" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="126" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>